<commit_message>
Add new feature and update existing components
</commit_message>
<xml_diff>
--- a/backend/Expense.xlsx
+++ b/backend/Expense.xlsx
@@ -418,35 +418,35 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>icons2</v>
+        <v>https://cdn.jsdelivr.net/npm/emoji-datasource-apple/img/apple/64/1f386.png</v>
       </c>
       <c r="C2">
-        <v>5000</v>
+        <v>1233</v>
       </c>
       <c r="D2" t="str">
-        <v>4/23/2025</v>
+        <v>5/30/2025</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>https://cdn.jsdelivr.net/npm/emoji-datasource-apple/img/apple/64/1f977.png</v>
+        <v>icons2</v>
       </c>
       <c r="C3">
-        <v>3331</v>
+        <v>5000</v>
       </c>
       <c r="D3" t="str">
-        <v>4/15/2025</v>
+        <v>4/23/2025</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>https://cdn.jsdelivr.net/npm/emoji-datasource-apple/img/apple/64/1f3e7.png</v>
+        <v>https://cdn.jsdelivr.net/npm/emoji-datasource-apple/img/apple/64/1f977.png</v>
       </c>
       <c r="C4">
-        <v>12333</v>
+        <v>3331</v>
       </c>
       <c r="D4" t="str">
-        <v>4/7/2025</v>
+        <v>4/15/2025</v>
       </c>
     </row>
     <row r="5">

</xml_diff>